<commit_message>
afternoon material on normalization, views, indices, procedures
</commit_message>
<xml_diff>
--- a/week12/day04/normalization examples.xlsx
+++ b/week12/day04/normalization examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehicks\SkillStorm\jon_javavettec20221003\100322-VET-TEC-Java\week12\day04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40016A16-B5DD-4118-B498-24D183D1DD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C482DA-7F4A-4834-91F7-89D454CD40F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{34CBD774-C7FC-4444-976B-A5D26E48C688}"/>
+    <workbookView xWindow="34515" yWindow="2910" windowWidth="17280" windowHeight="9060" firstSheet="1" activeTab="5" xr2:uid="{34CBD774-C7FC-4444-976B-A5D26E48C688}"/>
   </bookViews>
   <sheets>
     <sheet name="Normalization" sheetId="5" r:id="rId1"/>
@@ -1545,16 +1545,21 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1600"/>
-            <a:t>What is 1NF?</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t>What is 1NF? first normal form = must</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t> have a primary key, and no repeating groups/</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1600"/>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="en-US" sz="1600"/>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1600"/>
-            <a:t>What is 2NF?</a:t>
+            <a:t>What is 2NF? must be in 1NF, and have no partial dependencies</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1563,8 +1568,21 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1600"/>
-            <a:t>What is 3NF?</a:t>
-          </a:r>
+            <a:t>What is 3NF? must be in 2NF,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>must</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t> not have transitive dependencies</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1600"/>
@@ -1597,7 +1615,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>" "</a:t>
+            <a:t>" the KEY</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>, the WHOLE KEY, and nothing but the KEY. So help me Codd.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>"</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4248,8 +4290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3C69A3-0D98-45EB-8499-B4DEE7A7DBB8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>